<commit_message>
version v2.0.2 changed regulator to 7808
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gospar\Documents\Altium\ArduinoFOC\Project Outputs for ArduinoFOC\SimpleFOCShieldV2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gospar\Documents\github\Arduino-SimpleFOCShield\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -230,10 +230,10 @@
     <t>L1</t>
   </si>
   <si>
-    <t>L7805</t>
-  </si>
-  <si>
     <t>0.01Ohm 2512</t>
+  </si>
+  <si>
+    <t>L7808</t>
   </si>
 </sst>
 </file>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +841,7 @@
         <v>56</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>57</v>
@@ -882,7 +882,7 @@
         <v>67</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="3">

</xml_diff>

<commit_message>
added the updated bom and pick and place bugfix #11
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gospar\Documents\Altium\ArduinoFOC\Project Outputs for ArduinoFOC\ShieldVersions\SimpleFOCShieldV2.0.4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gospar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="ArduinoFOC" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>Designator</t>
   </si>
@@ -228,13 +228,16 @@
   </si>
   <si>
     <t xml:space="preserve"> 2kOhm 1210</t>
+  </si>
+  <si>
+    <t>Footprint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +256,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -300,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -311,6 +321,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -595,7 +607,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,6 +634,9 @@
       <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -639,6 +654,9 @@
       <c r="E2" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="F2" s="6">
+        <v>1206</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -656,6 +674,9 @@
       <c r="E3" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="F3" s="6">
+        <v>1206</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -673,6 +694,9 @@
       <c r="E4" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="F4" s="6">
+        <v>1206</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -690,6 +714,9 @@
       <c r="E5" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="F5" s="6">
+        <v>1206</v>
+      </c>
       <c r="L5" t="s">
         <v>20</v>
       </c>
@@ -710,6 +737,9 @@
       <c r="E6" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="F6" s="6">
+        <v>1206</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -726,6 +756,9 @@
       </c>
       <c r="E7" s="2" t="s">
         <v>29</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -744,6 +777,9 @@
       <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="F8" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -761,6 +797,9 @@
       <c r="E9" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="F9" s="6">
+        <v>1206</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -778,6 +817,9 @@
       <c r="E10" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="F10" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -795,6 +837,9 @@
       <c r="E11" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="F11" s="6">
+        <v>1210</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -812,6 +857,9 @@
       <c r="E12" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="F12" s="6">
+        <v>1210</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -829,6 +877,9 @@
       <c r="E13" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="F13" s="6">
+        <v>1206</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -844,6 +895,9 @@
         <v>2</v>
       </c>
       <c r="E14" s="2"/>
+      <c r="F14" s="7">
+        <v>2510</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -859,6 +913,9 @@
         <v>1</v>
       </c>
       <c r="E15" s="2"/>
+      <c r="F15" s="6">
+        <v>1206</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -872,8 +929,11 @@
         <v>2</v>
       </c>
       <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>60</v>
       </c>
@@ -885,8 +945,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>53</v>
       </c>
@@ -902,8 +965,11 @@
       <c r="E18" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
@@ -919,8 +985,11 @@
       <c r="E19" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>52</v>
       </c>
@@ -936,8 +1005,11 @@
       <c r="E20" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -953,8 +1025,11 @@
       <c r="E21" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -970,8 +1045,11 @@
       <c r="E22" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -986,6 +1064,9 @@
       </c>
       <c r="E23" s="2" t="s">
         <v>29</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>